<commit_message>
Updated the Python script as per the comments
</commit_message>
<xml_diff>
--- a/Utilities/names_mapping.xlsx
+++ b/Utilities/names_mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ChangeNames\07082019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{832F34CD-31AA-4576-A831-B99625AD8DA6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{482A8E30-8121-4B50-97F5-0A0F16D4A05F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1650" windowWidth="28800" windowHeight="13890" xr2:uid="{05871DF0-9518-41AA-8003-118BBCB396F6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{05871DF0-9518-41AA-8003-118BBCB396F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Names_Mapping" sheetId="4" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="bn" sheetId="2" r:id="rId3"/>
     <sheet name="ur" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3900" uniqueCount="1230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3908" uniqueCount="1233">
   <si>
     <t>en_old</t>
   </si>
@@ -3724,6 +3726,15 @@
   </si>
   <si>
     <t>en_bn_new</t>
+  </si>
+  <si>
+    <t>डॉसन</t>
+  </si>
+  <si>
+    <t>लुसी</t>
+  </si>
+  <si>
+    <t>June</t>
   </si>
 </sst>
 </file>
@@ -3745,12 +3756,18 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -3765,10 +3782,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4134,10 +4152,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90540321-5F96-4E73-82EE-73DFB728479C}">
-  <dimension ref="A1:Y129"/>
+  <dimension ref="A1:Y130"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AA8" sqref="AA8"/>
+    <sheetView tabSelected="1" topLeftCell="G35" workbookViewId="0">
+      <selection activeCell="U54" sqref="U54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4576,8 +4594,8 @@
       <c r="F9" t="s">
         <v>33</v>
       </c>
-      <c r="H9" t="s">
-        <v>34</v>
+      <c r="H9" s="3" t="s">
+        <v>819</v>
       </c>
       <c r="I9" t="s">
         <v>35</v>
@@ -7124,19 +7142,19 @@
         <v>245</v>
       </c>
       <c r="B63" t="s">
-        <v>246</v>
+        <v>317</v>
       </c>
       <c r="E63" t="s">
         <v>245</v>
       </c>
       <c r="F63" t="s">
-        <v>246</v>
-      </c>
-      <c r="H63" t="s">
-        <v>247</v>
+        <v>317</v>
+      </c>
+      <c r="H63" s="3" t="s">
+        <v>1230</v>
       </c>
       <c r="I63" t="s">
-        <v>248</v>
+        <v>319</v>
       </c>
       <c r="L63" t="s">
         <v>245</v>
@@ -9796,8 +9814,8 @@
       <c r="F120" t="s">
         <v>468</v>
       </c>
-      <c r="H120" t="s">
-        <v>469</v>
+      <c r="H120" s="3" t="s">
+        <v>1231</v>
       </c>
       <c r="I120" t="s">
         <v>470</v>
@@ -10269,6 +10287,32 @@
       </c>
       <c r="Y129" t="s">
         <v>1224</v>
+      </c>
+    </row>
+    <row r="130" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>1232</v>
+      </c>
+      <c r="B130" t="s">
+        <v>476</v>
+      </c>
+      <c r="E130" t="s">
+        <v>1232</v>
+      </c>
+      <c r="F130" t="s">
+        <v>476</v>
+      </c>
+      <c r="L130" t="s">
+        <v>1232</v>
+      </c>
+      <c r="M130" t="s">
+        <v>476</v>
+      </c>
+      <c r="R130" t="s">
+        <v>1232</v>
+      </c>
+      <c r="S130" t="s">
+        <v>1198</v>
       </c>
     </row>
   </sheetData>
@@ -10276,6 +10320,7 @@
     <hyperlink ref="I104" r:id="rId1" display="https://hi.wikipedia.org/wiki/%E0%A4%A8%E0%A4%BF%E0%A4%B0%E0%A5%8D%E0%A4%AE%E0%A4%B2%E0%A4%BE_(%E0%A4%89%E0%A4%AA%E0%A4%A8%E0%A5%8D%E0%A4%AF%E0%A4%BE%E0%A4%B8)" xr:uid="{7553EE3A-1126-4FC6-B291-3B9B17942D18}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>